<commit_message>
i guess final commit before defending task
</commit_message>
<xml_diff>
--- a/map_visualizer/тип_маршрутов.xlsx
+++ b/map_visualizer/тип_маршрутов.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>расстояние между концами 6181 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 6181 м</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>расстояние между концами 6181 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 6181 м</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>расстояние между концами 18895 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 18895 м</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>расстояние между концами 18895 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 18895 м</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>расстояние между концами 11450 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 11450 м</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>расстояние между концами 11450 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 11450 м</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>расстояние между концами 18895 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 18895 м</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>расстояние между концами 18895 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 18895 м</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>расстояние между концами 13747 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13747 м</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>расстояние между концами 13278 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 13278 м</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>расстояние между концами 15372 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 15372 м</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>расстояние между концами 15196 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 15196 м</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>расстояние между концами 5583 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 5583 м</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>расстояние между концами 5560 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 5560 м</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>расстояние между концами 11915 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 11915 м</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>расстояние между концами 12284 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 12284 м</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>расстояние между концами 12500 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 12500 м</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>расстояние между концами 13085 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 13085 м</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>найдено 8 резких поворотов &lt; 60°</t>
+          <t>8 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>найдено 6 резких поворотов &lt; 60°</t>
+          <t>6 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>найдено 8 резких поворотов &lt; 60°</t>
+          <t>8 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>расстояние между концами 10814 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 10814 м</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>расстояние между концами 7369 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 7369 м</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>расстояние между концами 7362 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 7362 м</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>расстояние между концами 10679 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10679 м</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>расстояние между концами 10702 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10702 м</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>расстояние между концами 14019 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 14019 м</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>расстояние между концами 14019 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 14019 м</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>расстояние между концами 12493 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 12493 м</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>расстояние между концами 12493 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 12493 м</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>расстояние между концами 14834 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 14834 м</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>расстояние между концами 14728 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 14728 м</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>расстояние между концами 10847 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10847 м</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>расстояние между концами 10847 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 10847 м</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>расстояние между концами 12656 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 12656 м</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>расстояние между концами 12656 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 12656 м</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>расстояние между концами 13291 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 13291 м</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>расстояние между концами 13291 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 13291 м</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>расстояние между концами 13291 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 13291 м</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>найдено 5 резких поворотов &lt; 60°</t>
+          <t>5 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>расстояние между концами 6995 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 6995 м</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>расстояние между концами 6995 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 6995 м</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>расстояние между концами 16263 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 16263 м</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>расстояние между концами 16263 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 16263 м</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>расстояние между концами 16792 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 16792 м</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>расстояние между концами 16757 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 16757 м</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>расстояние между концами 6348 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 6348 м</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>расстояние между концами 6348 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 6348 м</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>расстояние между концами 15268 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15268 м</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>расстояние между концами 15268 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 15268 м</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>расстояние между концами 13514 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 13514 м</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>расстояние между концами 13514 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 13514 м</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>расстояние между концами 7191 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 7191 м</t>
         </is>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>расстояние между концами 7194 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 7194 м</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>расстояние между концами 17063 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 17063 м</t>
         </is>
       </c>
     </row>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>расстояние между концами 17134 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 17134 м</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>найдено 7 резких поворотов &lt; 60°</t>
+          <t>7 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>найдено 7 резких поворотов &lt; 60°</t>
+          <t>7 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>расстояние между концами 12512 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 12512 м</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>расстояние между концами 12512 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 12512 м</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>расстояние между концами 9439 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 9439 м</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>расстояние между концами 9430 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 9430 м</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>расстояние между концами 18082 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 18082 м</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>расстояние между концами 18144 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 18144 м</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>расстояние между концами 19811 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 19811 м</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>расстояние между концами 19801 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 19801 м</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>расстояние между концами 22762 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 22762 м</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>расстояние между концами 22764 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 22764 м</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>найдено 5 резких поворотов &lt; 60°</t>
+          <t>5 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>расстояние между концами 31144 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 31144 м</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>расстояние между концами 17370 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 17370 м</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>расстояние между концами 17223 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 17223 м</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>расстояние между концами 19696 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 19696 м</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>расстояние между концами 19696 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 19696 м</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>расстояние между концами 30971 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 30971 м</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>расстояние между концами 30971 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 30971 м</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>расстояние между концами 34487 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 34487 м</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>расстояние между концами 34503 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 34503 м</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>расстояние между концами 10459 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 10459 м</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>расстояние между концами 10459 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10459 м</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>расстояние между концами 30021 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 30021 м</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>расстояние между концами 29872 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 29872 м</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>расстояние между концами 18490 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 18490 м</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>расстояние между концами 18338 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 18338 м</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>расстояние между концами 31144 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 31144 м</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>расстояние между концами 31144 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 31144 м</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>расстояние между концами 13682 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13682 м</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>расстояние между концами 13666 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13666 м</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>расстояние между концами 12810 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 12810 м</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>расстояние между концами 12786 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 12786 м</t>
         </is>
       </c>
     </row>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>расстояние между концами 59117 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 59117 м</t>
         </is>
       </c>
     </row>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>расстояние между концами 59112 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 59112 м</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>расстояние между концами 28972 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 28972 м</t>
         </is>
       </c>
     </row>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>расстояние между концами 28972 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 28972 м</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>расстояние между концами 27217 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 27217 м</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>расстояние между концами 27285 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 27285 м</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>расстояние между концами 16102 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 16102 м</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>расстояние между концами 16077 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 16077 м</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>расстояние между концами 10360 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 10360 м</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>расстояние между концами 10500 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 10500 м</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>расстояние между концами 17742 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 17742 м</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>расстояние между концами 17746 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 17746 м</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>расстояние между концами 15339 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15339 м</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>расстояние между концами 15339 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 15339 м</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>расстояние между концами 16113 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 16113 м</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>расстояние между концами 16119 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 16119 м</t>
         </is>
       </c>
     </row>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>найдено 6 резких поворотов &lt; 60°</t>
+          <t>6 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>расстояние между концами 24522 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 24522 м</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>расстояние между концами 15349 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15349 м</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>расстояние между концами 15339 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 15339 м</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>расстояние между концами 18500 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 18500 м</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>расстояние между концами 18352 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 18352 м</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>расстояние между концами 44040 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 44040 м</t>
         </is>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>расстояние между концами 44045 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 44045 м</t>
         </is>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>расстояние между концами 25287 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 25287 м</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>расстояние между концами 25287 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 25287 м</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>расстояние между концами 35807 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 35807 м</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>расстояние между концами 35824 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 35824 м</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>расстояние между концами 11495 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 11495 м</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>расстояние между концами 11459 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11459 м</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>расстояние между концами 13686 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 13686 м</t>
         </is>
       </c>
     </row>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>расстояние между концами 13892 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 13892 м</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>расстояние между концами 15077 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 15077 м</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>расстояние между концами 15077 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15077 м</t>
         </is>
       </c>
     </row>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>расстояние между концами 14260 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 14260 м</t>
         </is>
       </c>
     </row>
@@ -3223,7 +3223,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>расстояние между концами 15114 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 15114 м</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>расстояние между концами 9416 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 9416 м</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>расстояние между концами 9345 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 9345 м</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>расстояние между концами 15567 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15567 м</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>расстояние между концами 15567 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 15567 м</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>расстояние между концами 13465 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 13465 м</t>
         </is>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>расстояние между концами 13505 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 13505 м</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>расстояние между концами 9284 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 9284 м</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>расстояние между концами 9351 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 9351 м</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>расстояние между концами 16279 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 16279 м</t>
         </is>
       </c>
     </row>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>расстояние между концами 16282 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 16282 м</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>расстояние между концами 11717 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11717 м</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>расстояние между концами 11717 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 11717 м</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>расстояние между концами 10900 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10900 м</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>расстояние между концами 10900 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10900 м</t>
         </is>
       </c>
     </row>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>расстояние между концами 17973 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 17973 м</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>расстояние между концами 18089 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 18089 м</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>расстояние между концами 14920 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 14920 м</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>расстояние между концами 14917 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 14917 м</t>
         </is>
       </c>
     </row>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>расстояние между концами 10557 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 10557 м</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>расстояние между концами 10557 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 10557 м</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>расстояние между концами 12512 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 12512 м</t>
         </is>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>расстояние между концами 12512 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 12512 м</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>расстояние между концами 11782 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 11782 м</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>расстояние между концами 11689 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 11689 м</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>расстояние между концами 17374 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 17374 м</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>расстояние между концами 17374 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 17374 м</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>расстояние между концами 13645 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13645 м</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>расстояние между концами 13584 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13584 м</t>
         </is>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>расстояние между концами 13131 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 13131 м</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>расстояние между концами 13008 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13008 м</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>расстояние между концами 18565 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 18565 м</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>расстояние между концами 18565 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 18565 м</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>расстояние между концами 14349 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 14349 м</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>расстояние между концами 14349 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 14349 м</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>расстояние между концами 16744 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 16744 м</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>расстояние между концами 16746 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 16746 м</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>расстояние между концами 9100 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 9100 м</t>
         </is>
       </c>
     </row>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>расстояние между концами 9067 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 9067 м</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>расстояние между концами 12963 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 12963 м</t>
         </is>
       </c>
     </row>
@@ -4103,7 +4103,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>расстояние между концами 12942 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 12942 м</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>расстояние между концами 15405 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15405 м</t>
         </is>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>расстояние между концами 15376 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 15376 м</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>расстояние между концами 10279 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 10279 м</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>расстояние между концами 10279 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 10279 м</t>
         </is>
       </c>
     </row>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>расстояние между концами 14866 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 14866 м</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>расстояние между концами 14866 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 14866 м</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>расстояние между концами 14513 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 14513 м</t>
         </is>
       </c>
     </row>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>расстояние между концами 14518 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 14518 м</t>
         </is>
       </c>
     </row>
@@ -4323,7 +4323,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>расстояние между началом и концом 29 м</t>
+          <t>расстояние между концами 29 м</t>
         </is>
       </c>
     </row>
@@ -4367,7 +4367,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>расстояние между началом и концом 29 м</t>
+          <t>расстояние между концами 29 м</t>
         </is>
       </c>
     </row>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>расстояние между концами 10088 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10088 м</t>
         </is>
       </c>
     </row>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>расстояние между концами 10088 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10088 м</t>
         </is>
       </c>
     </row>
@@ -4433,7 +4433,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>расстояние между концами 10125 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 10125 м</t>
         </is>
       </c>
     </row>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>расстояние между концами 10125 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 10125 м</t>
         </is>
       </c>
     </row>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>расстояние между концами 13019 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 13019 м</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>расстояние между концами 12925 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 12925 м</t>
         </is>
       </c>
     </row>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>найдено 6 резких поворотов &lt; 60°</t>
+          <t>6 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>расстояние между концами 28031 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 28031 м</t>
         </is>
       </c>
     </row>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>расстояние между концами 13584 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13584 м</t>
         </is>
       </c>
     </row>
@@ -4587,7 +4587,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>расстояние между концами 13584 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 13584 м</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>расстояние между концами 6789 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 6789 м</t>
         </is>
       </c>
     </row>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>расстояние между концами 6789 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 6789 м</t>
         </is>
       </c>
     </row>
@@ -4653,7 +4653,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>расстояние между концами 3824 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 3824 м</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>найдено 5 резких поворотов &lt; 60°</t>
+          <t>5 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>расстояние между концами 8933 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 8933 м</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>расстояние между концами 8924 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 8924 м</t>
         </is>
       </c>
     </row>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>расстояние между концами 22068 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 22068 м</t>
         </is>
       </c>
     </row>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>расстояние между концами 22049 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 22049 м</t>
         </is>
       </c>
     </row>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>расстояние между концами 8502 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 8502 м</t>
         </is>
       </c>
     </row>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>расстояние между концами 8502 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 8502 м</t>
         </is>
       </c>
     </row>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>расстояние между концами 12404 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 12404 м</t>
         </is>
       </c>
     </row>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>расстояние между концами 12390 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 12390 м</t>
         </is>
       </c>
     </row>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>расстояние между концами 19873 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 19873 м</t>
         </is>
       </c>
     </row>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>расстояние между концами 19873 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 19873 м</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>расстояние между концами 9087 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 9087 м</t>
         </is>
       </c>
     </row>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>расстояние между концами 8960 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 8960 м</t>
         </is>
       </c>
     </row>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>расстояние между концами 10435 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 10435 м</t>
         </is>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>расстояние между концами 10316 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 10316 м</t>
         </is>
       </c>
     </row>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>расстояние между концами 11787 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11787 м</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>расстояние между концами 11680 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11680 м</t>
         </is>
       </c>
     </row>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>расстояние между концами 11670 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11670 м</t>
         </is>
       </c>
     </row>
@@ -5071,7 +5071,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>расстояние между концами 11713 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 11713 м</t>
         </is>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>расстояние между концами 16979 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 16979 м</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>расстояние между концами 16979 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 16979 м</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>расстояние между концами 11635 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 11635 м</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>найдено 5 резких поворотов &lt; 60°</t>
+          <t>5 острых углов &lt; 60°</t>
         </is>
       </c>
     </row>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>расстояние между концами 13620 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 13620 м</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>расстояние между концами 13514 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 13514 м</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>расстояние между концами 14674 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 14674 м</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>расстояние между концами 14674 м, поворотов: 1</t>
+          <t>1 поворотов, расстояние концов 14674 м</t>
         </is>
       </c>
     </row>
@@ -5269,7 +5269,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>расстояние между концами 14923 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 14923 м</t>
         </is>
       </c>
     </row>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>расстояние между концами 14920 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 14920 м</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>расстояние между концами 11855 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11855 м</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>расстояние между концами 11855 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 11855 м</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>расстояние между концами 10100 м, поворотов: 3</t>
+          <t>3 поворотов, расстояние концов 10100 м</t>
         </is>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>расстояние между концами 10208 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 10208 м</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>расстояние между концами 5153 м, поворотов: 2</t>
+          <t>2 поворотов, расстояние концов 5153 м</t>
         </is>
       </c>
     </row>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>расстояние между концами 5146 м, поворотов: 4</t>
+          <t>4 поворотов, расстояние концов 5146 м</t>
         </is>
       </c>
     </row>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>расстояние между концами 16174 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 16174 м</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>расстояние между концами 16174 м, поворотов: 0</t>
+          <t>0 поворотов, расстояние концов 16174 м</t>
         </is>
       </c>
     </row>

</xml_diff>